<commit_message>
Multiple changes: Excel modification, new 15 added to main (FFmpeg), 9 more started
</commit_message>
<xml_diff>
--- a/ExcelFiles/FFmpeg.xlsx
+++ b/ExcelFiles/FFmpeg.xlsx
@@ -5,22 +5,38 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muyeedahmed/Desktop/Gitcode/LLMVerification/Projects/FFmpeg/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muyeedahmed/Desktop/Gitcode/LLMVerification/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0F1BB9-5914-9748-B4EE-8DA56F3AE7E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849FAEA6-5AE2-BF48-B8B3-708AEE9EC782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="500" windowWidth="27440" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-48500" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$61</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="250">
   <si>
     <t>Commit Date</t>
   </si>
@@ -37,12 +53,12 @@
     <t>Changed Functions</t>
   </si>
   <si>
+    <t>LoC</t>
+  </si>
+  <si>
     <t>Line Changes</t>
   </si>
   <si>
-    <t>Message Len</t>
-  </si>
-  <si>
     <t>ChatGPT 4o</t>
   </si>
   <si>
@@ -55,37 +71,16 @@
     <t>New Function</t>
   </si>
   <si>
-    <t>TestSuite</t>
-  </si>
-  <si>
-    <t>2024-03-27</t>
-  </si>
-  <si>
-    <t>2024-04-01</t>
-  </si>
-  <si>
-    <t>2024-04-02</t>
-  </si>
-  <si>
-    <t>2024-04-07</t>
-  </si>
-  <si>
-    <t>2024-04-27</t>
-  </si>
-  <si>
-    <t>2022-04-09</t>
-  </si>
-  <si>
-    <t>2022-03-21</t>
-  </si>
-  <si>
-    <t>2022-03-22</t>
-  </si>
-  <si>
-    <t>2022-04-29</t>
-  </si>
-  <si>
-    <t>2022-02-25</t>
+    <t>llm_start</t>
+  </si>
+  <si>
+    <t>llm_end</t>
+  </si>
+  <si>
+    <t>orig_start</t>
+  </si>
+  <si>
+    <t>orig_end</t>
   </si>
   <si>
     <t>2d1c0dea5f6b91bec7f5fa53ec050913d851e366</t>
@@ -872,10 +867,7 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Test_Suite</t>
-  </si>
-  <si>
-    <t>LoC</t>
+    <t>Function LoC</t>
   </si>
 </sst>
 </file>
@@ -883,7 +875,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -937,12 +929,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1247,1988 +1245,2492 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M61"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A31" sqref="A31:A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>40939</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F2">
         <v>539</v>
       </c>
       <c r="G2">
+        <v>108</v>
+      </c>
+      <c r="H2">
         <v>11</v>
       </c>
-      <c r="H2">
-        <v>24</v>
-      </c>
       <c r="I2" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="J2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+      <c r="M2">
+        <v>81</v>
+      </c>
+      <c r="N2">
+        <v>189</v>
+      </c>
+      <c r="O2">
+        <v>81</v>
+      </c>
+      <c r="P2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>40939</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E3" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="F3">
         <v>540</v>
       </c>
       <c r="G3">
+        <v>57</v>
+      </c>
+      <c r="H3">
         <v>3</v>
       </c>
-      <c r="H3">
-        <v>39</v>
-      </c>
       <c r="I3" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+      <c r="M3">
+        <v>316</v>
+      </c>
+      <c r="N3">
+        <v>373</v>
+      </c>
+      <c r="O3">
+        <v>316</v>
+      </c>
+      <c r="P3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>41181</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E4" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="F4">
         <v>645</v>
       </c>
       <c r="G4">
+        <v>136</v>
+      </c>
+      <c r="H4">
         <v>6</v>
       </c>
-      <c r="H4">
-        <v>37</v>
-      </c>
       <c r="I4" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="J4" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="K4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+        <v>242</v>
+      </c>
+      <c r="M4">
+        <v>397</v>
+      </c>
+      <c r="N4">
+        <v>537</v>
+      </c>
+      <c r="O4">
+        <v>397</v>
+      </c>
+      <c r="P4">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>41618</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="E5" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="F5">
         <v>1785</v>
       </c>
       <c r="G5">
+        <v>153</v>
+      </c>
+      <c r="H5">
         <v>5</v>
       </c>
-      <c r="H5">
-        <v>18</v>
-      </c>
       <c r="I5" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+      <c r="M5">
+        <v>1286</v>
+      </c>
+      <c r="N5">
+        <v>1439</v>
+      </c>
+      <c r="O5">
+        <v>1282</v>
+      </c>
+      <c r="P5">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>41992</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E6" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F6">
         <v>327</v>
       </c>
       <c r="G6">
+        <v>122</v>
+      </c>
+      <c r="H6">
         <v>15</v>
       </c>
-      <c r="H6">
-        <v>28</v>
-      </c>
       <c r="I6" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J6" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="K6" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="L6" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+      <c r="M6">
+        <v>35</v>
+      </c>
+      <c r="N6">
+        <v>139</v>
+      </c>
+      <c r="O6">
+        <v>35</v>
+      </c>
+      <c r="P6">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>42059</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D7" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E7" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="F7">
         <v>2394</v>
       </c>
       <c r="G7">
+        <v>293</v>
+      </c>
+      <c r="H7">
         <v>2</v>
       </c>
-      <c r="H7">
-        <v>8</v>
-      </c>
       <c r="I7" t="s">
+        <v>231</v>
+      </c>
+      <c r="J7" t="s">
         <v>238</v>
       </c>
-      <c r="J7" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M7">
+        <v>345</v>
+      </c>
+      <c r="N7">
+        <v>635</v>
+      </c>
+      <c r="O7">
+        <v>325</v>
+      </c>
+      <c r="P7">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>42059</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D8" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E8" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="F8">
         <v>401</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>48</v>
       </c>
-      <c r="H8">
-        <v>11</v>
-      </c>
       <c r="I8" t="s">
+        <v>231</v>
+      </c>
+      <c r="J8" t="s">
         <v>238</v>
       </c>
-      <c r="J8" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>42059</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D9" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E9" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="F9">
         <v>2394</v>
       </c>
       <c r="G9">
+        <v>23</v>
+      </c>
+      <c r="H9">
         <v>2</v>
       </c>
-      <c r="H9">
-        <v>8</v>
-      </c>
       <c r="I9" t="s">
+        <v>231</v>
+      </c>
+      <c r="J9" t="s">
         <v>238</v>
       </c>
-      <c r="J9" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M9">
+        <v>326</v>
+      </c>
+      <c r="N9">
+        <v>349</v>
+      </c>
+      <c r="O9">
+        <v>306</v>
+      </c>
+      <c r="P9">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>42063</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D10" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E10" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="F10">
         <v>65</v>
       </c>
       <c r="G10">
+        <v>64</v>
+      </c>
+      <c r="H10">
         <v>2</v>
       </c>
-      <c r="H10">
-        <v>8</v>
-      </c>
       <c r="I10" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J10" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="N10">
+        <v>71</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>42063</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D11" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E11" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="F11">
         <v>130</v>
       </c>
       <c r="G11">
+        <v>127</v>
+      </c>
+      <c r="H11">
         <v>10</v>
       </c>
-      <c r="H11">
-        <v>7</v>
-      </c>
       <c r="I11" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="J11" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>132</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>42065</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D12" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="E12" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="F12">
         <v>958</v>
       </c>
       <c r="G12">
+        <v>116</v>
+      </c>
+      <c r="H12">
         <v>4</v>
       </c>
-      <c r="H12">
-        <v>8</v>
-      </c>
       <c r="I12" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="J12" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+      <c r="M12">
+        <v>412</v>
+      </c>
+      <c r="N12">
+        <v>528</v>
+      </c>
+      <c r="O12">
+        <v>412</v>
+      </c>
+      <c r="P12">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>42065</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D13" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E13" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="F13">
         <v>3528</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>44</v>
       </c>
-      <c r="H13">
-        <v>8</v>
-      </c>
       <c r="I13" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="J13" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>42067</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D14" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E14" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F14">
         <v>295</v>
       </c>
       <c r="G14">
+        <v>15</v>
+      </c>
+      <c r="H14">
         <v>1</v>
       </c>
-      <c r="H14">
-        <v>10</v>
-      </c>
       <c r="I14" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J14" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+      <c r="M14">
+        <v>265</v>
+      </c>
+      <c r="N14">
+        <v>279</v>
+      </c>
+      <c r="O14">
+        <v>267</v>
+      </c>
+      <c r="P14">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>42067</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D15" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E15" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F15">
         <v>200</v>
       </c>
       <c r="G15">
+        <v>131</v>
+      </c>
+      <c r="H15">
         <v>2</v>
       </c>
-      <c r="H15">
-        <v>4</v>
-      </c>
       <c r="I15" t="s">
+        <v>232</v>
+      </c>
+      <c r="J15" t="s">
         <v>239</v>
       </c>
-      <c r="J15" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M15">
+        <v>60</v>
+      </c>
+      <c r="N15">
+        <v>191</v>
+      </c>
+      <c r="O15">
+        <v>59</v>
+      </c>
+      <c r="P15">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>42068</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D16" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E16" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="F16">
         <v>293</v>
       </c>
       <c r="G16">
+        <v>114</v>
+      </c>
+      <c r="H16">
         <v>2</v>
       </c>
-      <c r="H16">
-        <v>4</v>
-      </c>
       <c r="I16" t="s">
+        <v>232</v>
+      </c>
+      <c r="J16" t="s">
+        <v>236</v>
+      </c>
+      <c r="M16">
+        <v>145</v>
+      </c>
+      <c r="N16">
         <v>239</v>
       </c>
-      <c r="J16" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O16">
+        <v>161</v>
+      </c>
+      <c r="P16">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>42068</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D17" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="E17" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="F17">
         <v>1476</v>
       </c>
       <c r="G17">
+        <v>198</v>
+      </c>
+      <c r="H17">
         <v>5</v>
       </c>
-      <c r="H17">
-        <v>6</v>
-      </c>
       <c r="I17" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J17" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+      <c r="M17">
+        <v>576</v>
+      </c>
+      <c r="N17">
+        <v>785</v>
+      </c>
+      <c r="O17">
+        <v>576</v>
+      </c>
+      <c r="P17">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>42068</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D18" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E18" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="F18">
         <v>802</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>7</v>
       </c>
-      <c r="H18">
-        <v>6</v>
-      </c>
       <c r="I18" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="J18" t="s">
-        <v>243</v>
-      </c>
-      <c r="M18" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>42069</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D19" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="E19" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="F19">
         <v>985</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>27</v>
       </c>
-      <c r="H19">
-        <v>6</v>
-      </c>
       <c r="I19" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="J19" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>42069</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D20" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="E20" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="F20">
         <v>958</v>
       </c>
       <c r="G20">
+        <v>154</v>
+      </c>
+      <c r="H20">
         <v>2</v>
       </c>
-      <c r="H20">
-        <v>8</v>
-      </c>
       <c r="I20" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="J20" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+      <c r="M20">
+        <v>512</v>
+      </c>
+      <c r="N20">
+        <v>666</v>
+      </c>
+      <c r="O20">
+        <v>512</v>
+      </c>
+      <c r="P20">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>42071</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D21" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E21" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="F21">
         <v>1777</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>30</v>
       </c>
-      <c r="H21">
-        <v>7</v>
-      </c>
       <c r="I21" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="J21" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>42071</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D22" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E22" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="F22">
         <v>979</v>
       </c>
       <c r="G22">
+        <v>73</v>
+      </c>
+      <c r="H22">
         <v>2</v>
       </c>
-      <c r="H22">
-        <v>6</v>
-      </c>
       <c r="I22" t="s">
+        <v>231</v>
+      </c>
+      <c r="J22" t="s">
         <v>238</v>
       </c>
-      <c r="J22" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M22">
+        <v>278</v>
+      </c>
+      <c r="N22">
+        <v>351</v>
+      </c>
+      <c r="O22">
+        <v>278</v>
+      </c>
+      <c r="P22">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>42071</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D23" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E23" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="F23">
         <v>1779</v>
       </c>
       <c r="G23">
+        <v>55</v>
+      </c>
+      <c r="H23">
         <v>7</v>
       </c>
-      <c r="H23">
-        <v>6</v>
-      </c>
       <c r="I23" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J23" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+      <c r="M23">
+        <v>1287</v>
+      </c>
+      <c r="N23">
+        <v>1339</v>
+      </c>
+      <c r="O23">
+        <v>1287</v>
+      </c>
+      <c r="P23">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>42071</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D24" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E24" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="F24">
         <v>981</v>
       </c>
       <c r="G24">
+        <v>115</v>
+      </c>
+      <c r="H24">
         <v>2</v>
       </c>
-      <c r="H24">
-        <v>5</v>
-      </c>
       <c r="I24" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="J24" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+      <c r="M24">
+        <v>561</v>
+      </c>
+      <c r="N24">
+        <v>680</v>
+      </c>
+      <c r="O24">
+        <v>561</v>
+      </c>
+      <c r="P24">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>42072</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D25" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E25" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="F25">
         <v>566</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>4</v>
       </c>
-      <c r="H25">
-        <v>5</v>
-      </c>
       <c r="I25" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="J25" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>42387</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D26" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E26" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="F26">
         <v>362</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>7</v>
       </c>
-      <c r="H26">
-        <v>25</v>
-      </c>
       <c r="I26" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J26" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>43757</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D27" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E27" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="F27">
         <v>172</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>8</v>
       </c>
-      <c r="H27">
-        <v>7</v>
-      </c>
       <c r="I27" t="s">
+        <v>232</v>
+      </c>
+      <c r="J27" t="s">
         <v>239</v>
       </c>
-      <c r="J27" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>43757</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D28" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="E28" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="F28">
         <v>1066</v>
       </c>
       <c r="G28">
+        <v>44</v>
+      </c>
+      <c r="H28">
         <v>2</v>
       </c>
-      <c r="H28">
-        <v>14</v>
-      </c>
       <c r="I28" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J28" t="s">
-        <v>246</v>
-      </c>
-      <c r="M28" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+      <c r="M28">
+        <v>919</v>
+      </c>
+      <c r="N28">
+        <v>963</v>
+      </c>
+      <c r="O28">
+        <v>917</v>
+      </c>
+      <c r="P28">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>44345</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D29" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E29" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="F29">
         <v>7382</v>
       </c>
       <c r="G29">
+        <v>196</v>
+      </c>
+      <c r="H29">
         <v>6</v>
       </c>
-      <c r="H29">
-        <v>21</v>
-      </c>
       <c r="I29" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="J29" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+      <c r="M29">
+        <v>2087</v>
+      </c>
+      <c r="N29">
+        <v>2283</v>
+      </c>
+      <c r="O29">
+        <v>2087</v>
+      </c>
+      <c r="P29">
+        <v>2283</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>45204</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C30" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D30" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E30" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="F30">
         <v>1509</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>23</v>
       </c>
-      <c r="H30">
-        <v>123</v>
-      </c>
       <c r="I30" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J30" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>45804</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C31" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D31" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="E31" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="F31">
         <v>1255</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>8</v>
       </c>
-      <c r="H31">
-        <v>7</v>
-      </c>
       <c r="I31" t="s">
+        <v>231</v>
+      </c>
+      <c r="J31" t="s">
         <v>238</v>
       </c>
-      <c r="J31" t="s">
-        <v>245</v>
-      </c>
-      <c r="M31" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>45805</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D32" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E32" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="F32">
         <v>1036</v>
       </c>
       <c r="G32">
+        <v>53</v>
+      </c>
+      <c r="H32">
         <v>3</v>
       </c>
-      <c r="H32">
-        <v>5</v>
-      </c>
       <c r="I32" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="J32" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+      <c r="M32">
+        <v>309</v>
+      </c>
+      <c r="N32">
+        <v>366</v>
+      </c>
+      <c r="O32">
+        <v>309</v>
+      </c>
+      <c r="P32">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>45807</v>
       </c>
       <c r="B33" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D33" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E33" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="F33">
         <v>944</v>
       </c>
       <c r="G33">
+        <v>13</v>
+      </c>
+      <c r="H33">
         <v>37</v>
       </c>
-      <c r="H33">
-        <v>7</v>
-      </c>
       <c r="I33" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="J33" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+      <c r="M33">
+        <v>246</v>
+      </c>
+      <c r="N33">
+        <v>259</v>
+      </c>
+      <c r="O33">
+        <v>246</v>
+      </c>
+      <c r="P33">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>45807</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C34" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D34" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E34" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="F34">
         <v>942</v>
       </c>
       <c r="G34">
+        <v>194</v>
+      </c>
+      <c r="H34">
         <v>4</v>
       </c>
-      <c r="H34">
-        <v>6</v>
-      </c>
       <c r="I34" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J34" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+      <c r="M34">
+        <v>54</v>
+      </c>
+      <c r="N34">
+        <v>248</v>
+      </c>
+      <c r="O34">
+        <v>54</v>
+      </c>
+      <c r="P34">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>45808</v>
       </c>
       <c r="B35" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C35" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D35" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E35" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="F35">
         <v>3087</v>
       </c>
       <c r="G35">
+        <v>43</v>
+      </c>
+      <c r="H35">
         <v>3</v>
       </c>
-      <c r="H35">
-        <v>6</v>
-      </c>
       <c r="I35" t="s">
+        <v>231</v>
+      </c>
+      <c r="J35" t="s">
         <v>238</v>
       </c>
-      <c r="J35" t="s">
-        <v>245</v>
-      </c>
-      <c r="M35" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M35">
+        <v>348</v>
+      </c>
+      <c r="N35">
+        <v>394</v>
+      </c>
+      <c r="O35">
+        <v>348</v>
+      </c>
+      <c r="P35">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>45808</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C36" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D36" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="E36" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="F36">
         <v>121</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>66</v>
       </c>
-      <c r="H36">
-        <v>3</v>
-      </c>
       <c r="I36" t="s">
+        <v>231</v>
+      </c>
+      <c r="J36" t="s">
         <v>238</v>
       </c>
-      <c r="J36" t="s">
-        <v>245</v>
-      </c>
       <c r="K36" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="L36" t="s">
-        <v>255</v>
-      </c>
-      <c r="M36" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>45808</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C37" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D37" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E37" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="F37">
         <v>683</v>
       </c>
       <c r="G37">
+        <v>94</v>
+      </c>
+      <c r="H37">
         <v>3</v>
       </c>
-      <c r="H37">
-        <v>9</v>
-      </c>
       <c r="I37" t="s">
+        <v>231</v>
+      </c>
+      <c r="J37" t="s">
         <v>238</v>
       </c>
-      <c r="J37" t="s">
-        <v>245</v>
-      </c>
-      <c r="M37" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M37">
+        <v>223</v>
+      </c>
+      <c r="N37">
+        <v>317</v>
+      </c>
+      <c r="O37">
+        <v>222</v>
+      </c>
+      <c r="P37">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>45808</v>
       </c>
       <c r="B38" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C38" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D38" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="E38" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F38">
         <v>167</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>27</v>
       </c>
-      <c r="H38">
-        <v>3</v>
-      </c>
       <c r="I38" t="s">
+        <v>231</v>
+      </c>
+      <c r="J38" t="s">
         <v>238</v>
       </c>
-      <c r="J38" t="s">
-        <v>245</v>
-      </c>
       <c r="L38" t="s">
-        <v>255</v>
-      </c>
-      <c r="M38" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>45808</v>
       </c>
       <c r="B39" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C39" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D39" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E39" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F39">
         <v>1259</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>14</v>
       </c>
-      <c r="H39">
-        <v>6</v>
-      </c>
       <c r="I39" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J39" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="K39" t="s">
-        <v>252</v>
-      </c>
-      <c r="M39" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>45808</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C40" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D40" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E40" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F40">
         <v>8948</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>4</v>
       </c>
-      <c r="H40">
-        <v>7</v>
-      </c>
       <c r="I40" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="J40" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>45809</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C41" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D41" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E41" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="F41">
         <v>8948</v>
       </c>
       <c r="G41">
+        <v>221</v>
+      </c>
+      <c r="H41">
         <v>2</v>
       </c>
-      <c r="H41">
-        <v>6</v>
-      </c>
       <c r="I41" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="J41" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+      <c r="M41">
+        <v>6332</v>
+      </c>
+      <c r="N41">
+        <v>6553</v>
+      </c>
+      <c r="O41">
+        <v>6332</v>
+      </c>
+      <c r="P41">
+        <v>6553</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>45810</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C42" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D42" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E42" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="F42">
         <v>199</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>37</v>
       </c>
-      <c r="H42">
-        <v>6</v>
-      </c>
       <c r="I42" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J42" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>45810</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C43" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D43" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="F43">
         <v>196</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <v>5</v>
       </c>
-      <c r="H43">
-        <v>6</v>
-      </c>
       <c r="I43" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="J43" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>45810</v>
       </c>
       <c r="B44" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C44" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D44" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E44" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="F44">
         <v>708</v>
       </c>
       <c r="G44">
+        <v>44</v>
+      </c>
+      <c r="H44">
         <v>33</v>
       </c>
-      <c r="H44">
-        <v>6</v>
-      </c>
       <c r="I44" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J44" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="K44" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+      <c r="M44">
+        <v>660</v>
+      </c>
+      <c r="N44">
+        <v>702</v>
+      </c>
+      <c r="O44">
+        <v>659</v>
+      </c>
+      <c r="P44">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>45810</v>
       </c>
       <c r="B45" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C45" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D45" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E45" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="F45">
         <v>243</v>
       </c>
       <c r="G45">
+        <v>44</v>
+      </c>
+      <c r="H45">
         <v>3</v>
       </c>
-      <c r="H45">
-        <v>20</v>
-      </c>
       <c r="I45" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="J45" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>12</v>
+        <v>241</v>
+      </c>
+      <c r="M45">
+        <v>157</v>
+      </c>
+      <c r="N45">
+        <v>201</v>
+      </c>
+      <c r="O45">
+        <v>157</v>
+      </c>
+      <c r="P45">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>45378</v>
       </c>
       <c r="B46" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C46" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D46" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="E46" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="F46">
         <v>971</v>
       </c>
       <c r="G46">
+        <v>250</v>
+      </c>
+      <c r="H46">
         <v>5</v>
       </c>
       <c r="I46" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J46" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>13</v>
+        <v>240</v>
+      </c>
+      <c r="M46">
+        <v>145</v>
+      </c>
+      <c r="N46">
+        <v>392</v>
+      </c>
+      <c r="O46">
+        <v>145</v>
+      </c>
+      <c r="P46">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>45383</v>
       </c>
       <c r="B47" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C47" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D47" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E47" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="F47">
         <v>10299</v>
       </c>
       <c r="G47">
+        <v>88</v>
+      </c>
+      <c r="H47">
         <v>10</v>
       </c>
       <c r="I47" t="s">
+        <v>231</v>
+      </c>
+      <c r="J47" t="s">
         <v>238</v>
       </c>
-      <c r="J47" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>14</v>
+      <c r="M47">
+        <v>9367</v>
+      </c>
+      <c r="N47">
+        <v>9398</v>
+      </c>
+      <c r="O47">
+        <v>9367</v>
+      </c>
+      <c r="P47">
+        <v>9455</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>45384</v>
       </c>
       <c r="B48" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C48" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D48" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E48" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="F48">
         <v>10301</v>
       </c>
       <c r="G48">
+        <v>49</v>
+      </c>
+      <c r="H48">
         <v>1</v>
       </c>
       <c r="I48" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J48" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>14</v>
+        <v>236</v>
+      </c>
+      <c r="M48">
+        <v>5010</v>
+      </c>
+      <c r="N48">
+        <v>5059</v>
+      </c>
+      <c r="O48">
+        <v>5010</v>
+      </c>
+      <c r="P48">
+        <v>5059</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>45384</v>
       </c>
       <c r="B49" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C49" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D49" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="E49" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="F49">
         <v>454</v>
       </c>
       <c r="G49">
+        <v>54</v>
+      </c>
+      <c r="H49">
         <v>8</v>
       </c>
       <c r="I49" t="s">
+        <v>231</v>
+      </c>
+      <c r="J49" t="s">
         <v>238</v>
       </c>
-      <c r="J49" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>14</v>
+      <c r="M49">
+        <v>327</v>
+      </c>
+      <c r="N49">
+        <v>375</v>
+      </c>
+      <c r="O49">
+        <v>327</v>
+      </c>
+      <c r="P49">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <v>45384</v>
       </c>
       <c r="B50" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C50" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D50" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E50" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="F50">
         <v>10302</v>
       </c>
       <c r="G50">
+        <v>50</v>
+      </c>
+      <c r="H50">
         <v>1</v>
       </c>
       <c r="I50" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J50" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>14</v>
+        <v>236</v>
+      </c>
+      <c r="M50">
+        <v>5010</v>
+      </c>
+      <c r="N50">
+        <v>5037</v>
+      </c>
+      <c r="O50">
+        <v>5010</v>
+      </c>
+      <c r="P50">
+        <v>5060</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>45384</v>
       </c>
       <c r="B51" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C51" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D51" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E51" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="F51">
         <v>10300</v>
       </c>
       <c r="G51">
+        <v>48</v>
+      </c>
+      <c r="H51">
         <v>3</v>
       </c>
       <c r="I51" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J51" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>14</v>
+        <v>236</v>
+      </c>
+      <c r="M51">
+        <v>5010</v>
+      </c>
+      <c r="N51">
+        <v>5055</v>
+      </c>
+      <c r="O51">
+        <v>5010</v>
+      </c>
+      <c r="P51">
+        <v>5058</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <v>45384</v>
       </c>
       <c r="B52" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C52" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D52" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E52" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="F52">
         <v>10302</v>
       </c>
       <c r="G52">
+        <v>51</v>
+      </c>
+      <c r="H52">
         <v>2</v>
       </c>
       <c r="I52" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J52" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>14</v>
+        <v>236</v>
+      </c>
+      <c r="M52">
+        <v>5010</v>
+      </c>
+      <c r="N52">
+        <v>5060</v>
+      </c>
+      <c r="O52">
+        <v>5010</v>
+      </c>
+      <c r="P52">
+        <v>5061</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>45384</v>
       </c>
       <c r="B53" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C53" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D53" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E53" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="F53">
         <v>1183</v>
       </c>
       <c r="G53">
+        <v>48</v>
+      </c>
+      <c r="H53">
         <v>3</v>
       </c>
       <c r="I53" t="s">
+        <v>231</v>
+      </c>
+      <c r="J53" t="s">
         <v>238</v>
       </c>
-      <c r="J53" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>14</v>
+      <c r="M53">
+        <v>255</v>
+      </c>
+      <c r="N53">
+        <v>310</v>
+      </c>
+      <c r="O53">
+        <v>255</v>
+      </c>
+      <c r="P53">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>45384</v>
       </c>
       <c r="B54" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C54" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D54" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E54" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F54">
         <v>10299</v>
       </c>
       <c r="G54">
+        <v>107</v>
+      </c>
+      <c r="H54">
         <v>2</v>
       </c>
       <c r="I54" t="s">
+        <v>231</v>
+      </c>
+      <c r="J54" t="s">
         <v>238</v>
       </c>
-      <c r="J54" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>15</v>
+      <c r="M54">
+        <v>8783</v>
+      </c>
+      <c r="N54">
+        <v>8850</v>
+      </c>
+      <c r="O54">
+        <v>8783</v>
+      </c>
+      <c r="P54">
+        <v>8890</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>45389</v>
       </c>
       <c r="B55" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C55" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D55" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E55" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="F55">
         <v>1360</v>
       </c>
       <c r="G55">
+        <v>54</v>
+      </c>
+      <c r="H55">
         <v>8</v>
       </c>
       <c r="I55" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J55" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>16</v>
+        <v>240</v>
+      </c>
+      <c r="M55">
+        <v>270</v>
+      </c>
+      <c r="N55">
+        <v>323</v>
+      </c>
+      <c r="O55">
+        <v>270</v>
+      </c>
+      <c r="P55">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>45409</v>
       </c>
       <c r="B56" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C56" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D56" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E56" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="F56">
         <v>10319</v>
       </c>
       <c r="G56">
+        <v>96</v>
+      </c>
+      <c r="H56">
         <v>3</v>
       </c>
       <c r="I56" t="s">
+        <v>231</v>
+      </c>
+      <c r="J56" t="s">
         <v>238</v>
       </c>
-      <c r="J56" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>17</v>
+      <c r="M56">
+        <v>9382</v>
+      </c>
+      <c r="N56">
+        <v>9443</v>
+      </c>
+      <c r="O56">
+        <v>9382</v>
+      </c>
+      <c r="P56">
+        <v>9478</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>44660</v>
       </c>
       <c r="B57" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C57" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D57" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E57" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="F57">
         <v>3449</v>
       </c>
       <c r="G57">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="H57">
         <v>6</v>
       </c>
       <c r="I57" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="J57" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>18</v>
+        <v>236</v>
+      </c>
+      <c r="M57">
+        <v>2648</v>
+      </c>
+      <c r="N57">
+        <v>2744</v>
+      </c>
+      <c r="O57">
+        <v>2648</v>
+      </c>
+      <c r="P57">
+        <v>2746</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
+        <v>44641</v>
       </c>
       <c r="B58" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C58" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D58" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E58" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="F58">
         <v>2135</v>
       </c>
       <c r="G58">
-        <v>2</v>
+        <v>270</v>
       </c>
       <c r="H58">
         <v>2</v>
       </c>
       <c r="I58" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J58" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>19</v>
+        <v>240</v>
+      </c>
+      <c r="M58">
+        <v>320</v>
+      </c>
+      <c r="N58">
+        <v>606</v>
+      </c>
+      <c r="O58">
+        <v>320</v>
+      </c>
+      <c r="P58">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <v>44642</v>
       </c>
       <c r="B59" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C59" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D59" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E59" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F59">
         <v>7516</v>
       </c>
       <c r="G59">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="H59">
         <v>5</v>
       </c>
       <c r="I59" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="J59" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>20</v>
+        <v>236</v>
+      </c>
+      <c r="M59">
+        <v>5609</v>
+      </c>
+      <c r="N59">
+        <v>5656</v>
+      </c>
+      <c r="O59">
+        <v>5609</v>
+      </c>
+      <c r="P59">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
+        <v>44680</v>
       </c>
       <c r="B60" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C60" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D60" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E60" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="F60">
         <v>482</v>
       </c>
       <c r="G60">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="H60">
         <v>10</v>
       </c>
       <c r="I60" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="J60" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>21</v>
+        <v>239</v>
+      </c>
+      <c r="M60">
+        <v>387</v>
+      </c>
+      <c r="N60">
+        <v>475</v>
+      </c>
+      <c r="O60">
+        <v>387</v>
+      </c>
+      <c r="P60">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A61" s="2">
+        <v>44617</v>
       </c>
       <c r="B61" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C61" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D61" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E61" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F61">
         <v>389</v>
       </c>
       <c r="G61">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="H61">
         <v>2</v>
       </c>
       <c r="I61" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="J61" t="s">
-        <v>246</v>
+        <v>239</v>
+      </c>
+      <c r="M61">
+        <v>314</v>
+      </c>
+      <c r="N61">
+        <v>354</v>
+      </c>
+      <c r="O61">
+        <v>314</v>
+      </c>
+      <c r="P61">
+        <v>353</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:P61" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Excelfile update with the new 19 commits
</commit_message>
<xml_diff>
--- a/ExcelFiles/FFmpeg.xlsx
+++ b/ExcelFiles/FFmpeg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muyeedahmed/Desktop/Gitcode/LLMVerification/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849FAEA6-5AE2-BF48-B8B3-708AEE9EC782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74390FCD-EFBF-B74C-9436-446569AD3F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48500" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="500" windowWidth="27440" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="326">
   <si>
     <t>Commit Date</t>
   </si>
@@ -786,9 +786,6 @@
   </si>
   <si>
     <t>Same Error</t>
-  </si>
-  <si>
-    <t>Kl</t>
   </si>
   <si>
     <t>libavcodec/gifdec.c:125:18: error: 'break' statement not in loop or switch statement
@@ -868,6 +865,237 @@
   </si>
   <si>
     <t>Function LoC</t>
+  </si>
+  <si>
+    <t>01f63ef0b44fa70d87edaf52f19fcdb2ae7446b3</t>
+  </si>
+  <si>
+    <t>fftools/ffmpeg_filter: also remove display matrix side data from buffered frames</t>
+  </si>
+  <si>
+    <t>fftools/ffmpeg_filter.c</t>
+  </si>
+  <si>
+    <t>configure_filtergraph</t>
+  </si>
+  <si>
+    <t>0af1d69959696aa4baab7feef361e57d62f2e3f4</t>
+  </si>
+  <si>
+    <t>avcodec/hevc/hevcdec: move the slice header buffer overread check up in the function</t>
+  </si>
+  <si>
+    <t>libavcodec/hevc/hevcdec.c</t>
+  </si>
+  <si>
+    <t>hls_slice_header</t>
+  </si>
+  <si>
+    <t>No Change (Wrong diff)</t>
+  </si>
+  <si>
+    <t>0c1d87d1e61cbb0f0ffa0d95d9e8b77d5bbde70a</t>
+  </si>
+  <si>
+    <t>swscale/swscale_unscaled: fix packed30togbra10() for formats with bpc between 9-14 bits</t>
+  </si>
+  <si>
+    <t>libswscale/swscale_unscaled.c</t>
+  </si>
+  <si>
+    <t>packed30togbra10</t>
+  </si>
+  <si>
+    <t>1c170613975d3cbcbb5aaa469b4a3cf0df5d4c2b</t>
+  </si>
+  <si>
+    <t>avcodec/decode: Fix avcodec parameters when bsfs are enable by decoder</t>
+  </si>
+  <si>
+    <t>libavcodec/decode.c</t>
+  </si>
+  <si>
+    <t>decode_bsfs_init</t>
+  </si>
+  <si>
+    <t>20502ba92a5936bc6a6e006d05828b750f4290ed</t>
+  </si>
+  <si>
+    <t>ffmpeg: Don't print graphs if there are no outputs yet</t>
+  </si>
+  <si>
+    <t>Partial Fix (Logic)</t>
+  </si>
+  <si>
+    <t>3fa70c03e4bf0eb2661324305dce48795a5b9c8d</t>
+  </si>
+  <si>
+    <t>avformat/iamf_writer: be more verbose when reporting an input layout is invalid</t>
+  </si>
+  <si>
+    <t>libavformat/iamf_writer.c</t>
+  </si>
+  <si>
+    <t>ff_iamf_add_audio_element</t>
+  </si>
+  <si>
+    <t>4bf784c0e5615c3f934e677d5de093a8be7da7ae</t>
+  </si>
+  <si>
+    <t>avformat/dump: print only the actual streams in a tile grid group</t>
+  </si>
+  <si>
+    <t>libavformat/dump.c</t>
+  </si>
+  <si>
+    <t>dump_stream_group</t>
+  </si>
+  <si>
+    <t>Wrong (Removed Code)</t>
+  </si>
+  <si>
+    <t>Syntax Error</t>
+  </si>
+  <si>
+    <t>5150d26e0af2041fd4a8df4ec6f56e59a672fa62</t>
+  </si>
+  <si>
+    <t>checkasm: hevc sao_edge, benchmarking inside the width loop is meaningless</t>
+  </si>
+  <si>
+    <t>tests/checkasm/hevc_sao.c</t>
+  </si>
+  <si>
+    <t>check_sao_edge</t>
+  </si>
+  <si>
+    <t>5470d024e18968b3bdef2b745966f7617f1eb9f2</t>
+  </si>
+  <si>
+    <t>avformat/iamf_parse: ensure there's at most one of each parameter types in audio elements</t>
+  </si>
+  <si>
+    <t>libavformat/iamf_parse.c</t>
+  </si>
+  <si>
+    <t>audio_element_obu</t>
+  </si>
+  <si>
+    <t>5ca14b23f1e8137258580dd9045f025795b2eb88</t>
+  </si>
+  <si>
+    <t>avcodec/ffv1dec: compute end instead of hardcoding it and test for fltmap correctly</t>
+  </si>
+  <si>
+    <t>libavcodec/ffv1dec.c</t>
+  </si>
+  <si>
+    <t>decode_remap</t>
+  </si>
+  <si>
+    <t>748e960e04248569d121ac4ebba11109b6c81acb</t>
+  </si>
+  <si>
+    <t>swscale/swscale_unscaled: fix packed16togbra16() for formats with bpc between 9-14 bits</t>
+  </si>
+  <si>
+    <t>packed16togbra16</t>
+  </si>
+  <si>
+    <t>89df6d40689aad113383e74299928b647e46905e</t>
+  </si>
+  <si>
+    <t>avcodec/ffv1enc: Fix remap &gt; 0 with gbrp12, that is non float</t>
+  </si>
+  <si>
+    <t>libavcodec/ffv1enc.c</t>
+  </si>
+  <si>
+    <t>ff_ffv1_encode_setup_plane_info</t>
+  </si>
+  <si>
+    <t>94beaf48723adb01d452fddaa99f384350ed5c41</t>
+  </si>
+  <si>
+    <t>avcodec/videotoolboxenc: Add AYUV as a candidate pix_fmt for HEVC alpha</t>
+  </si>
+  <si>
+    <t>libavcodec/videotoolboxenc.c</t>
+  </si>
+  <si>
+    <t>vtenc_create_encoder</t>
+  </si>
+  <si>
+    <t>No Change (Wrong diff - rearranged lines)</t>
+  </si>
+  <si>
+    <t>98d97bb33b2a54265b3d41838b2fb64310360e22</t>
+  </si>
+  <si>
+    <t>rtmp: Set correct message stream id when writing as server</t>
+  </si>
+  <si>
+    <t>libavformat/rtmpproto.c</t>
+  </si>
+  <si>
+    <t>rtmp_write</t>
+  </si>
+  <si>
+    <t>9e12572933dc1c49e9b35d772ddcae896c2ba8a8</t>
+  </si>
+  <si>
+    <t>avformat/hls: .ts is always ok even if its a mov/mp4</t>
+  </si>
+  <si>
+    <t>libavformat/hls.c</t>
+  </si>
+  <si>
+    <t>test_segment</t>
+  </si>
+  <si>
+    <t>2919767750da9acc9042fcc2b8fa3e134cfd16c9</t>
+  </si>
+  <si>
+    <t>Revert "avformat/dump: print only the actual streams in a tile grid group"</t>
+  </si>
+  <si>
+    <t>Similar Warning</t>
+  </si>
+  <si>
+    <t>49726a922fd2b358feb7753488d415180da5121c</t>
+  </si>
+  <si>
+    <t>avfilter/vf_scale: remove global side data when it no longer applies after scaling</t>
+  </si>
+  <si>
+    <t>libavfilter/vf_scale.c</t>
+  </si>
+  <si>
+    <t>config_props</t>
+  </si>
+  <si>
+    <t>670089304ac856f01591c88bbb7c115d423935da</t>
+  </si>
+  <si>
+    <t>lavc/vvc: Avoid UB in DB strength derivation for PLT CUs</t>
+  </si>
+  <si>
+    <t>libavcodec/vvc/filter.c</t>
+  </si>
+  <si>
+    <t>boundary_strength</t>
+  </si>
+  <si>
+    <t>b9b4c9ebf07748993ad91ba9b9b9f06914d67865</t>
+  </si>
+  <si>
+    <t>avcodec/get_buffer: Use av_buffer_mallocz() for audio same as its done for video</t>
+  </si>
+  <si>
+    <t>libavcodec/get_buffer.c</t>
+  </si>
+  <si>
+    <t>update_frame_pool</t>
   </si>
 </sst>
 </file>
@@ -1245,17 +1473,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P61"/>
+  <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:A43"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
     <col min="5" max="5" width="56.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -1278,7 +1508,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>6</v>
@@ -1427,9 +1657,6 @@
       <c r="J4" t="s">
         <v>236</v>
       </c>
-      <c r="K4" t="s">
-        <v>242</v>
-      </c>
       <c r="M4">
         <v>397</v>
       </c>
@@ -1519,10 +1746,10 @@
         <v>237</v>
       </c>
       <c r="K6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M6">
         <v>35</v>
@@ -2692,10 +2919,10 @@
         <v>238</v>
       </c>
       <c r="K36" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L36" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
@@ -2771,7 +2998,7 @@
         <v>238</v>
       </c>
       <c r="L38" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
@@ -2803,7 +3030,7 @@
         <v>237</v>
       </c>
       <c r="K39" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
@@ -2966,7 +3193,7 @@
         <v>237</v>
       </c>
       <c r="K44" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="M44">
         <v>660</v>
@@ -3727,6 +3954,846 @@
       </c>
       <c r="P61">
         <v>353</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A62" s="2">
+        <v>45719</v>
+      </c>
+      <c r="B62" t="s">
+        <v>249</v>
+      </c>
+      <c r="C62" t="s">
+        <v>250</v>
+      </c>
+      <c r="D62" t="s">
+        <v>251</v>
+      </c>
+      <c r="E62" t="s">
+        <v>252</v>
+      </c>
+      <c r="F62">
+        <v>3200</v>
+      </c>
+      <c r="G62">
+        <v>176</v>
+      </c>
+      <c r="H62">
+        <v>4</v>
+      </c>
+      <c r="I62" t="s">
+        <v>231</v>
+      </c>
+      <c r="J62" t="s">
+        <v>236</v>
+      </c>
+      <c r="M62">
+        <v>1898</v>
+      </c>
+      <c r="N62">
+        <v>2076</v>
+      </c>
+      <c r="O62">
+        <v>1898</v>
+      </c>
+      <c r="P62">
+        <v>2074</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A63" s="2">
+        <v>45782</v>
+      </c>
+      <c r="B63" t="s">
+        <v>253</v>
+      </c>
+      <c r="C63" t="s">
+        <v>254</v>
+      </c>
+      <c r="D63" t="s">
+        <v>255</v>
+      </c>
+      <c r="E63" t="s">
+        <v>256</v>
+      </c>
+      <c r="F63">
+        <v>4230</v>
+      </c>
+      <c r="G63">
+        <v>451</v>
+      </c>
+      <c r="H63">
+        <v>12</v>
+      </c>
+      <c r="I63" t="s">
+        <v>257</v>
+      </c>
+      <c r="J63" t="s">
+        <v>236</v>
+      </c>
+      <c r="M63">
+        <v>739</v>
+      </c>
+      <c r="N63">
+        <v>1190</v>
+      </c>
+      <c r="O63">
+        <v>739</v>
+      </c>
+      <c r="P63">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A64" s="2">
+        <v>45800</v>
+      </c>
+      <c r="B64" t="s">
+        <v>258</v>
+      </c>
+      <c r="C64" t="s">
+        <v>259</v>
+      </c>
+      <c r="D64" t="s">
+        <v>260</v>
+      </c>
+      <c r="E64" t="s">
+        <v>261</v>
+      </c>
+      <c r="F64">
+        <v>2705</v>
+      </c>
+      <c r="G64">
+        <v>80</v>
+      </c>
+      <c r="H64">
+        <v>5</v>
+      </c>
+      <c r="I64" t="s">
+        <v>231</v>
+      </c>
+      <c r="J64" t="s">
+        <v>236</v>
+      </c>
+      <c r="M64">
+        <v>803</v>
+      </c>
+      <c r="N64">
+        <v>883</v>
+      </c>
+      <c r="O64">
+        <v>803</v>
+      </c>
+      <c r="P64">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A65" s="2">
+        <v>45752</v>
+      </c>
+      <c r="B65" t="s">
+        <v>262</v>
+      </c>
+      <c r="C65" t="s">
+        <v>263</v>
+      </c>
+      <c r="D65" t="s">
+        <v>264</v>
+      </c>
+      <c r="E65" t="s">
+        <v>265</v>
+      </c>
+      <c r="F65">
+        <v>2223</v>
+      </c>
+      <c r="G65">
+        <v>38</v>
+      </c>
+      <c r="H65">
+        <v>3</v>
+      </c>
+      <c r="I65" t="s">
+        <v>233</v>
+      </c>
+      <c r="J65" t="s">
+        <v>236</v>
+      </c>
+      <c r="M65">
+        <v>174</v>
+      </c>
+      <c r="N65">
+        <v>217</v>
+      </c>
+      <c r="O65">
+        <v>174</v>
+      </c>
+      <c r="P65">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A66" s="2">
+        <v>45795</v>
+      </c>
+      <c r="B66" t="s">
+        <v>266</v>
+      </c>
+      <c r="C66" t="s">
+        <v>267</v>
+      </c>
+      <c r="D66" t="s">
+        <v>158</v>
+      </c>
+      <c r="E66" t="s">
+        <v>205</v>
+      </c>
+      <c r="F66">
+        <v>1033</v>
+      </c>
+      <c r="G66">
+        <v>53</v>
+      </c>
+      <c r="H66">
+        <v>2</v>
+      </c>
+      <c r="I66" t="s">
+        <v>268</v>
+      </c>
+      <c r="J66" t="s">
+        <v>236</v>
+      </c>
+      <c r="M66">
+        <v>309</v>
+      </c>
+      <c r="N66">
+        <v>364</v>
+      </c>
+      <c r="O66">
+        <v>309</v>
+      </c>
+      <c r="P66">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A67" s="2">
+        <v>45660</v>
+      </c>
+      <c r="B67" t="s">
+        <v>269</v>
+      </c>
+      <c r="C67" t="s">
+        <v>270</v>
+      </c>
+      <c r="D67" t="s">
+        <v>271</v>
+      </c>
+      <c r="E67" t="s">
+        <v>272</v>
+      </c>
+      <c r="F67">
+        <v>1183</v>
+      </c>
+      <c r="G67">
+        <v>191</v>
+      </c>
+      <c r="H67">
+        <v>9</v>
+      </c>
+      <c r="I67" t="s">
+        <v>231</v>
+      </c>
+      <c r="J67" t="s">
+        <v>236</v>
+      </c>
+      <c r="M67">
+        <v>193</v>
+      </c>
+      <c r="N67">
+        <v>386</v>
+      </c>
+      <c r="O67">
+        <v>193</v>
+      </c>
+      <c r="P67">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A68" s="2">
+        <v>45660</v>
+      </c>
+      <c r="B68" t="s">
+        <v>273</v>
+      </c>
+      <c r="C68" t="s">
+        <v>274</v>
+      </c>
+      <c r="D68" t="s">
+        <v>275</v>
+      </c>
+      <c r="E68" t="s">
+        <v>276</v>
+      </c>
+      <c r="F68">
+        <v>927</v>
+      </c>
+      <c r="G68">
+        <v>173</v>
+      </c>
+      <c r="H68">
+        <v>4</v>
+      </c>
+      <c r="I68" t="s">
+        <v>277</v>
+      </c>
+      <c r="J68" t="s">
+        <v>278</v>
+      </c>
+      <c r="M68">
+        <v>662</v>
+      </c>
+      <c r="N68">
+        <v>828</v>
+      </c>
+      <c r="O68">
+        <v>662</v>
+      </c>
+      <c r="P68">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A69" s="2">
+        <v>45791</v>
+      </c>
+      <c r="B69" t="s">
+        <v>279</v>
+      </c>
+      <c r="C69" t="s">
+        <v>280</v>
+      </c>
+      <c r="D69" t="s">
+        <v>281</v>
+      </c>
+      <c r="E69" t="s">
+        <v>282</v>
+      </c>
+      <c r="F69">
+        <v>160</v>
+      </c>
+      <c r="G69">
+        <v>44</v>
+      </c>
+      <c r="H69">
+        <v>14</v>
+      </c>
+      <c r="I69" t="s">
+        <v>231</v>
+      </c>
+      <c r="J69" t="s">
+        <v>239</v>
+      </c>
+      <c r="M69">
+        <v>95</v>
+      </c>
+      <c r="N69">
+        <v>139</v>
+      </c>
+      <c r="O69">
+        <v>95</v>
+      </c>
+      <c r="P69">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A70" s="2">
+        <v>45707</v>
+      </c>
+      <c r="B70" t="s">
+        <v>283</v>
+      </c>
+      <c r="C70" t="s">
+        <v>284</v>
+      </c>
+      <c r="D70" t="s">
+        <v>285</v>
+      </c>
+      <c r="E70" t="s">
+        <v>286</v>
+      </c>
+      <c r="F70">
+        <v>1143</v>
+      </c>
+      <c r="G70">
+        <v>174</v>
+      </c>
+      <c r="H70">
+        <v>14</v>
+      </c>
+      <c r="I70" t="s">
+        <v>231</v>
+      </c>
+      <c r="J70" t="s">
+        <v>278</v>
+      </c>
+      <c r="M70">
+        <v>617</v>
+      </c>
+      <c r="N70">
+        <v>809</v>
+      </c>
+      <c r="O70">
+        <v>617</v>
+      </c>
+      <c r="P70">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A71" s="2">
+        <v>45741</v>
+      </c>
+      <c r="B71" t="s">
+        <v>287</v>
+      </c>
+      <c r="C71" t="s">
+        <v>288</v>
+      </c>
+      <c r="D71" t="s">
+        <v>289</v>
+      </c>
+      <c r="E71" t="s">
+        <v>290</v>
+      </c>
+      <c r="F71">
+        <v>967</v>
+      </c>
+      <c r="G71">
+        <v>67</v>
+      </c>
+      <c r="H71">
+        <v>4</v>
+      </c>
+      <c r="I71" t="s">
+        <v>268</v>
+      </c>
+      <c r="J71" t="s">
+        <v>236</v>
+      </c>
+      <c r="M71">
+        <v>278</v>
+      </c>
+      <c r="N71">
+        <v>340</v>
+      </c>
+      <c r="O71">
+        <v>278</v>
+      </c>
+      <c r="P71">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A72" s="2">
+        <v>45800</v>
+      </c>
+      <c r="B72" t="s">
+        <v>291</v>
+      </c>
+      <c r="C72" t="s">
+        <v>292</v>
+      </c>
+      <c r="D72" t="s">
+        <v>260</v>
+      </c>
+      <c r="E72" t="s">
+        <v>293</v>
+      </c>
+      <c r="F72">
+        <v>2706</v>
+      </c>
+      <c r="G72">
+        <v>142</v>
+      </c>
+      <c r="H72">
+        <v>8</v>
+      </c>
+      <c r="I72" t="s">
+        <v>231</v>
+      </c>
+      <c r="J72" t="s">
+        <v>278</v>
+      </c>
+      <c r="M72">
+        <v>670</v>
+      </c>
+      <c r="N72">
+        <v>812</v>
+      </c>
+      <c r="O72">
+        <v>670</v>
+      </c>
+      <c r="P72">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A73" s="2">
+        <v>45754</v>
+      </c>
+      <c r="B73" t="s">
+        <v>294</v>
+      </c>
+      <c r="C73" t="s">
+        <v>295</v>
+      </c>
+      <c r="D73" t="s">
+        <v>296</v>
+      </c>
+      <c r="E73" t="s">
+        <v>297</v>
+      </c>
+      <c r="F73">
+        <v>1932</v>
+      </c>
+      <c r="G73">
+        <v>175</v>
+      </c>
+      <c r="H73">
+        <v>2</v>
+      </c>
+      <c r="I73" t="s">
+        <v>257</v>
+      </c>
+      <c r="J73" t="s">
+        <v>236</v>
+      </c>
+      <c r="M73">
+        <v>787</v>
+      </c>
+      <c r="N73">
+        <v>962</v>
+      </c>
+      <c r="O73">
+        <v>787</v>
+      </c>
+      <c r="P73">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A74" s="2">
+        <v>45733</v>
+      </c>
+      <c r="B74" t="s">
+        <v>298</v>
+      </c>
+      <c r="C74" t="s">
+        <v>299</v>
+      </c>
+      <c r="D74" t="s">
+        <v>300</v>
+      </c>
+      <c r="E74" t="s">
+        <v>301</v>
+      </c>
+      <c r="F74">
+        <v>3076</v>
+      </c>
+      <c r="G74">
+        <v>465</v>
+      </c>
+      <c r="H74">
+        <v>7</v>
+      </c>
+      <c r="I74" t="s">
+        <v>302</v>
+      </c>
+      <c r="J74" t="s">
+        <v>236</v>
+      </c>
+      <c r="M74">
+        <v>1166</v>
+      </c>
+      <c r="N74">
+        <v>1631</v>
+      </c>
+      <c r="O74">
+        <v>1166</v>
+      </c>
+      <c r="P74">
+        <v>1631</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A75" s="2">
+        <v>45714</v>
+      </c>
+      <c r="B75" t="s">
+        <v>303</v>
+      </c>
+      <c r="C75" t="s">
+        <v>304</v>
+      </c>
+      <c r="D75" t="s">
+        <v>305</v>
+      </c>
+      <c r="E75" t="s">
+        <v>306</v>
+      </c>
+      <c r="F75">
+        <v>3199</v>
+      </c>
+      <c r="G75">
+        <v>146</v>
+      </c>
+      <c r="H75">
+        <v>7</v>
+      </c>
+      <c r="I75" t="s">
+        <v>231</v>
+      </c>
+      <c r="J75" t="s">
+        <v>236</v>
+      </c>
+      <c r="M75">
+        <v>2991</v>
+      </c>
+      <c r="N75">
+        <v>3137</v>
+      </c>
+      <c r="O75">
+        <v>2988</v>
+      </c>
+      <c r="P75">
+        <v>3134</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A76" s="2">
+        <v>45690</v>
+      </c>
+      <c r="B76" t="s">
+        <v>307</v>
+      </c>
+      <c r="C76" t="s">
+        <v>308</v>
+      </c>
+      <c r="D76" t="s">
+        <v>309</v>
+      </c>
+      <c r="E76" t="s">
+        <v>310</v>
+      </c>
+      <c r="F76">
+        <v>2665</v>
+      </c>
+      <c r="G76">
+        <v>50</v>
+      </c>
+      <c r="H76">
+        <v>4</v>
+      </c>
+      <c r="I76" t="s">
+        <v>231</v>
+      </c>
+      <c r="J76" t="s">
+        <v>240</v>
+      </c>
+      <c r="M76">
+        <v>717</v>
+      </c>
+      <c r="N76">
+        <v>772</v>
+      </c>
+      <c r="O76">
+        <v>717</v>
+      </c>
+      <c r="P76">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A77" s="2">
+        <v>45662</v>
+      </c>
+      <c r="B77" t="s">
+        <v>311</v>
+      </c>
+      <c r="C77" t="s">
+        <v>312</v>
+      </c>
+      <c r="D77" t="s">
+        <v>275</v>
+      </c>
+      <c r="E77" t="s">
+        <v>276</v>
+      </c>
+      <c r="F77">
+        <v>927</v>
+      </c>
+      <c r="G77">
+        <f>P77-O77</f>
+        <v>173</v>
+      </c>
+      <c r="H77">
+        <v>12</v>
+      </c>
+      <c r="I77" t="s">
+        <v>231</v>
+      </c>
+      <c r="J77" t="s">
+        <v>313</v>
+      </c>
+      <c r="M77">
+        <v>662</v>
+      </c>
+      <c r="N77">
+        <v>828</v>
+      </c>
+      <c r="O77">
+        <v>662</v>
+      </c>
+      <c r="P77">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A78" s="2">
+        <v>45691</v>
+      </c>
+      <c r="B78" t="s">
+        <v>314</v>
+      </c>
+      <c r="C78" t="s">
+        <v>315</v>
+      </c>
+      <c r="D78" t="s">
+        <v>316</v>
+      </c>
+      <c r="E78" t="s">
+        <v>317</v>
+      </c>
+      <c r="F78">
+        <v>1292</v>
+      </c>
+      <c r="G78">
+        <f>P78-O78</f>
+        <v>92</v>
+      </c>
+      <c r="H78">
+        <v>10</v>
+      </c>
+      <c r="I78" t="s">
+        <v>231</v>
+      </c>
+      <c r="J78" t="s">
+        <v>313</v>
+      </c>
+      <c r="M78">
+        <v>622</v>
+      </c>
+      <c r="N78">
+        <v>714</v>
+      </c>
+      <c r="O78">
+        <v>622</v>
+      </c>
+      <c r="P78">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A79" s="2">
+        <v>45801</v>
+      </c>
+      <c r="B79" t="s">
+        <v>318</v>
+      </c>
+      <c r="C79" t="s">
+        <v>319</v>
+      </c>
+      <c r="D79" t="s">
+        <v>320</v>
+      </c>
+      <c r="E79" t="s">
+        <v>321</v>
+      </c>
+      <c r="F79">
+        <v>1247</v>
+      </c>
+      <c r="G79">
+        <f>P79-O79</f>
+        <v>96</v>
+      </c>
+      <c r="H79">
+        <v>3</v>
+      </c>
+      <c r="I79" t="s">
+        <v>257</v>
+      </c>
+      <c r="J79" t="s">
+        <v>239</v>
+      </c>
+      <c r="M79">
+        <v>354</v>
+      </c>
+      <c r="N79">
+        <v>450</v>
+      </c>
+      <c r="O79">
+        <v>354</v>
+      </c>
+      <c r="P79">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A80" s="2">
+        <v>45658</v>
+      </c>
+      <c r="B80" t="s">
+        <v>322</v>
+      </c>
+      <c r="C80" t="s">
+        <v>323</v>
+      </c>
+      <c r="D80" t="s">
+        <v>324</v>
+      </c>
+      <c r="E80" t="s">
+        <v>325</v>
+      </c>
+      <c r="F80">
+        <v>288</v>
+      </c>
+      <c r="G80">
+        <f>P80-O80</f>
+        <v>109</v>
+      </c>
+      <c r="H80">
+        <v>5</v>
+      </c>
+      <c r="I80" t="s">
+        <v>233</v>
+      </c>
+      <c r="J80" t="s">
+        <v>313</v>
+      </c>
+      <c r="M80">
+        <v>58</v>
+      </c>
+      <c r="N80">
+        <v>170</v>
+      </c>
+      <c r="O80">
+        <v>58</v>
+      </c>
+      <c r="P80">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added missing function sizes FFmpeg
</commit_message>
<xml_diff>
--- a/ExcelFiles/FFmpeg.xlsx
+++ b/ExcelFiles/FFmpeg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muyeedahmed/Desktop/Gitcode/LLMVerification/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF58376D-E27A-FB4F-A248-372EF9D4FFE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3AF125-F171-664E-9318-F6521A74E72E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-48500" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1427,8 +1427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G73" sqref="G73"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1786,7 +1786,7 @@
         <v>48</v>
       </c>
       <c r="I8" t="s">
-        <v>216</v>
+        <v>260</v>
       </c>
       <c r="J8" t="s">
         <v>222</v>
@@ -2922,7 +2922,7 @@
         <v>5</v>
       </c>
       <c r="I36" t="s">
-        <v>216</v>
+        <v>260</v>
       </c>
       <c r="J36" t="s">
         <v>224</v>
@@ -2966,7 +2966,7 @@
         <v>10</v>
       </c>
       <c r="I37" t="s">
-        <v>216</v>
+        <v>260</v>
       </c>
       <c r="J37" t="s">
         <v>222</v>
@@ -3098,7 +3098,7 @@
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>216</v>
+        <v>260</v>
       </c>
       <c r="J40" t="s">
         <v>220</v>
@@ -3274,7 +3274,7 @@
         <v>2</v>
       </c>
       <c r="I44" t="s">
-        <v>216</v>
+        <v>260</v>
       </c>
       <c r="J44" t="s">
         <v>222</v>
@@ -3362,7 +3362,7 @@
         <v>3</v>
       </c>
       <c r="I46" t="s">
-        <v>216</v>
+        <v>260</v>
       </c>
       <c r="J46" t="s">
         <v>222</v>

</xml_diff>

<commit_message>
FFmpeg clang report update
</commit_message>
<xml_diff>
--- a/ExcelFiles/FFmpeg.xlsx
+++ b/ExcelFiles/FFmpeg.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muyeedahmed/Desktop/Gitcode/LLMVerification/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3AF125-F171-664E-9318-F6521A74E72E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED55D7F-D3DE-5044-A140-6ABE139E2073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48500" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="500" windowWidth="27440" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$76</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1427,8 +1427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4681,11 +4681,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P60" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:P76" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P79">
       <sortCondition ref="A1:A79"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a new commit to FFmpeg
</commit_message>
<xml_diff>
--- a/ExcelFiles/FFmpeg.xlsx
+++ b/ExcelFiles/FFmpeg.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muyeedahmed/Desktop/Gitcode/LLMVerification/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED55D7F-D3DE-5044-A140-6ABE139E2073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FA468E-2B36-4349-B6EF-4B75C4FECA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="500" windowWidth="27440" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="-22640" windowWidth="27440" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$76</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="309">
   <si>
     <t>Commit Date</t>
   </si>
@@ -198,9 +198,6 @@
   </si>
   <si>
     <t>6f452ad1acadc50abc7d9b1b9d264e940a451ee7</t>
-  </si>
-  <si>
-    <t>83b34691429729fea2c78bf419622ceb4a7810b2</t>
   </si>
   <si>
     <t>fabf148578c0d628a9207de3b60aba57ac1c4bc3</t>
@@ -388,10 +385,6 @@
     <t>fftools/textformat/avtextformat: Fix races when initializing formatters</t>
   </si>
   <si>
-    <t>Fix Requirement: avcodec/x86/hpeldsp_init: Use ff_avg_pixels16_mmxext
- Give me the edited c file as attachment (Rename it &lt;filename&gt;_llm.c). Also show the diff.</t>
-  </si>
-  <si>
     <t>fftools/ffmpeg_enc: only promote first frame side data to global when meaningful</t>
   </si>
   <si>
@@ -527,9 +520,6 @@
     <t>fftools/textformat/avtextformat.c</t>
   </si>
   <si>
-    <t>libavcodec/x86/hpeldsp_init.c</t>
-  </si>
-  <si>
     <t>fftools/ffmpeg_enc.c</t>
   </si>
   <si>
@@ -668,9 +658,6 @@
     <t>formatters_register_all</t>
   </si>
   <si>
-    <t>hpeldsp_init_mmxext</t>
-  </si>
-  <si>
     <t>enc_open</t>
   </si>
   <si>
@@ -735,9 +722,6 @@
   </si>
   <si>
     <t>New Warnings</t>
-  </si>
-  <si>
-    <t>Same Error</t>
   </si>
   <si>
     <t>libavcodec/gifdec.c:125:18: error: 'break' statement not in loop or switch statement
@@ -1048,6 +1032,18 @@
   </si>
   <si>
     <t>read_distribution_bundle,read_vlc_prefix</t>
+  </si>
+  <si>
+    <t>c08d300481b8ebb846cd43a473988fdbc6793d1b</t>
+  </si>
+  <si>
+    <t>avformat/avformat: also clear FFFormatContext packet queue when closing a muxer</t>
+  </si>
+  <si>
+    <t>libavformat/avformat.c</t>
+  </si>
+  <si>
+    <t>avformat_free_context</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1105,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1120,6 +1116,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1427,7 +1426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E48" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
@@ -1460,7 +1459,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>6</v>
@@ -1498,13 +1497,13 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F2">
         <v>539</v>
@@ -1516,10 +1515,10 @@
         <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="J2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M2">
         <v>81</v>
@@ -1542,13 +1541,13 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F3">
         <v>540</v>
@@ -1560,10 +1559,10 @@
         <v>3</v>
       </c>
       <c r="I3" t="s">
+        <v>212</v>
+      </c>
+      <c r="J3" t="s">
         <v>216</v>
-      </c>
-      <c r="J3" t="s">
-        <v>220</v>
       </c>
       <c r="M3">
         <v>316</v>
@@ -1586,13 +1585,13 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F4">
         <v>645</v>
@@ -1604,10 +1603,10 @@
         <v>6</v>
       </c>
       <c r="I4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M4">
         <v>397</v>
@@ -1630,13 +1629,13 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F5">
         <v>1785</v>
@@ -1648,10 +1647,10 @@
         <v>5</v>
       </c>
       <c r="I5" t="s">
+        <v>212</v>
+      </c>
+      <c r="J5" t="s">
         <v>216</v>
-      </c>
-      <c r="J5" t="s">
-        <v>220</v>
       </c>
       <c r="M5">
         <v>1286</v>
@@ -1674,13 +1673,13 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F6">
         <v>327</v>
@@ -1692,16 +1691,16 @@
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J6" t="s">
+        <v>217</v>
+      </c>
+      <c r="K6" t="s">
         <v>221</v>
       </c>
-      <c r="K6" t="s">
-        <v>226</v>
-      </c>
       <c r="L6" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="M6">
         <v>35</v>
@@ -1724,13 +1723,13 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F7">
         <v>2394</v>
@@ -1742,10 +1741,10 @@
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J7" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="M7">
         <v>345</v>
@@ -1768,13 +1767,13 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E8" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F8">
         <v>401</v>
@@ -1786,10 +1785,10 @@
         <v>48</v>
       </c>
       <c r="I8" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J8" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="M8">
         <v>167</v>
@@ -1812,13 +1811,13 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F9">
         <v>2394</v>
@@ -1830,10 +1829,10 @@
         <v>2</v>
       </c>
       <c r="I9" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J9" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="M9">
         <v>326</v>
@@ -1856,13 +1855,13 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E10" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F10">
         <v>65</v>
@@ -1874,10 +1873,10 @@
         <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J10" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="M10">
         <v>2</v>
@@ -1900,13 +1899,13 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F11">
         <v>130</v>
@@ -1918,10 +1917,10 @@
         <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J11" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="M11">
         <v>1</v>
@@ -1944,13 +1943,13 @@
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E12" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F12">
         <v>958</v>
@@ -1962,10 +1961,10 @@
         <v>4</v>
       </c>
       <c r="I12" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J12" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M12">
         <v>412</v>
@@ -1988,13 +1987,13 @@
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E13" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F13">
         <v>3528</v>
@@ -2006,10 +2005,10 @@
         <v>44</v>
       </c>
       <c r="I13" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="J13" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
@@ -2020,13 +2019,13 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E14" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F14">
         <v>295</v>
@@ -2038,10 +2037,10 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J14" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="M14">
         <v>265</v>
@@ -2064,13 +2063,13 @@
         <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E15" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F15">
         <v>200</v>
@@ -2082,10 +2081,10 @@
         <v>2</v>
       </c>
       <c r="I15" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J15" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="M15">
         <v>60</v>
@@ -2108,13 +2107,13 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F16">
         <v>293</v>
@@ -2126,10 +2125,10 @@
         <v>2</v>
       </c>
       <c r="I16" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J16" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M16">
         <v>145</v>
@@ -2152,13 +2151,13 @@
         <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E17" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F17">
         <v>1476</v>
@@ -2170,10 +2169,10 @@
         <v>5</v>
       </c>
       <c r="I17" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J17" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="M17">
         <v>576</v>
@@ -2196,13 +2195,13 @@
         <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E18" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F18">
         <v>802</v>
@@ -2214,10 +2213,10 @@
         <v>7</v>
       </c>
       <c r="I18" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J18" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
@@ -2228,13 +2227,13 @@
         <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D19" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E19" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F19">
         <v>985</v>
@@ -2246,10 +2245,10 @@
         <v>27</v>
       </c>
       <c r="I19" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="J19" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
@@ -2260,13 +2259,13 @@
         <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E20" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F20">
         <v>958</v>
@@ -2278,10 +2277,10 @@
         <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J20" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M20">
         <v>512</v>
@@ -2304,13 +2303,13 @@
         <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E21" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F21">
         <v>1777</v>
@@ -2322,10 +2321,10 @@
         <v>30</v>
       </c>
       <c r="I21" t="s">
+        <v>213</v>
+      </c>
+      <c r="J21" t="s">
         <v>217</v>
-      </c>
-      <c r="J21" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
@@ -2336,13 +2335,13 @@
         <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E22" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F22">
         <v>979</v>
@@ -2354,10 +2353,10 @@
         <v>2</v>
       </c>
       <c r="I22" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J22" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="M22">
         <v>278</v>
@@ -2380,13 +2379,13 @@
         <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E23" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F23">
         <v>1779</v>
@@ -2398,10 +2397,10 @@
         <v>7</v>
       </c>
       <c r="I23" t="s">
+        <v>212</v>
+      </c>
+      <c r="J23" t="s">
         <v>216</v>
-      </c>
-      <c r="J23" t="s">
-        <v>220</v>
       </c>
       <c r="M23">
         <v>1287</v>
@@ -2424,13 +2423,13 @@
         <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E24" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F24">
         <v>981</v>
@@ -2442,10 +2441,10 @@
         <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="J24" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M24">
         <v>561</v>
@@ -2468,13 +2467,13 @@
         <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D25" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E25" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F25">
         <v>566</v>
@@ -2486,10 +2485,10 @@
         <v>4</v>
       </c>
       <c r="I25" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="J25" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
@@ -2500,13 +2499,13 @@
         <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D26" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E26" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F26">
         <v>362</v>
@@ -2518,10 +2517,10 @@
         <v>7</v>
       </c>
       <c r="I26" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J26" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
@@ -2532,13 +2531,13 @@
         <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D27" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E27" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F27">
         <v>172</v>
@@ -2550,10 +2549,10 @@
         <v>8</v>
       </c>
       <c r="I27" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J27" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
@@ -2564,13 +2563,13 @@
         <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D28" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E28" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F28">
         <v>1066</v>
@@ -2582,10 +2581,10 @@
         <v>2</v>
       </c>
       <c r="I28" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J28" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="M28">
         <v>919</v>
@@ -2608,13 +2607,13 @@
         <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D29" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E29" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F29">
         <v>7382</v>
@@ -2626,10 +2625,10 @@
         <v>6</v>
       </c>
       <c r="I29" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="J29" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M29">
         <v>2087</v>
@@ -2649,16 +2648,16 @@
         <v>44617</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D30" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E30" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F30">
         <v>389</v>
@@ -2670,10 +2669,10 @@
         <v>2</v>
       </c>
       <c r="I30" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="J30" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="M30">
         <v>314</v>
@@ -2693,16 +2692,16 @@
         <v>44641</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C31" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D31" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E31" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F31">
         <v>2135</v>
@@ -2714,10 +2713,10 @@
         <v>2</v>
       </c>
       <c r="I31" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J31" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="M31">
         <v>320</v>
@@ -2737,16 +2736,16 @@
         <v>44642</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D32" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E32" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="F32">
         <v>7516</v>
@@ -2758,10 +2757,10 @@
         <v>5</v>
       </c>
       <c r="I32" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="J32" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M32">
         <v>5609</v>
@@ -2781,16 +2780,16 @@
         <v>44660</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D33" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E33" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F33">
         <v>3449</v>
@@ -2802,10 +2801,10 @@
         <v>6</v>
       </c>
       <c r="I33" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="J33" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M33">
         <v>2648</v>
@@ -2825,16 +2824,16 @@
         <v>44680</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C34" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D34" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E34" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F34">
         <v>482</v>
@@ -2846,10 +2845,10 @@
         <v>10</v>
       </c>
       <c r="I34" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J34" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="M34">
         <v>387</v>
@@ -2872,13 +2871,13 @@
         <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D35" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E35" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="F35">
         <v>1509</v>
@@ -2890,10 +2889,10 @@
         <v>23</v>
       </c>
       <c r="I35" t="s">
+        <v>212</v>
+      </c>
+      <c r="J35" t="s">
         <v>216</v>
-      </c>
-      <c r="J35" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
@@ -2901,16 +2900,16 @@
         <v>45378</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C36" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D36" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E36" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F36">
         <v>971</v>
@@ -2922,10 +2921,10 @@
         <v>5</v>
       </c>
       <c r="I36" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J36" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="M36">
         <v>145</v>
@@ -2945,16 +2944,16 @@
         <v>45383</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C37" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D37" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E37" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F37">
         <v>10299</v>
@@ -2966,10 +2965,10 @@
         <v>10</v>
       </c>
       <c r="I37" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J37" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="M37">
         <v>9367</v>
@@ -2989,16 +2988,16 @@
         <v>45384</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D38" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E38" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F38">
         <v>10301</v>
@@ -3010,10 +3009,10 @@
         <v>1</v>
       </c>
       <c r="I38" t="s">
+        <v>212</v>
+      </c>
+      <c r="J38" t="s">
         <v>216</v>
-      </c>
-      <c r="J38" t="s">
-        <v>220</v>
       </c>
       <c r="M38">
         <v>5010</v>
@@ -3033,16 +3032,16 @@
         <v>45384</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C39" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D39" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E39" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F39">
         <v>454</v>
@@ -3054,10 +3053,10 @@
         <v>8</v>
       </c>
       <c r="I39" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J39" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="M39">
         <v>327</v>
@@ -3077,16 +3076,16 @@
         <v>45384</v>
       </c>
       <c r="B40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C40" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D40" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E40" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F40">
         <v>10302</v>
@@ -3098,10 +3097,10 @@
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J40" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M40">
         <v>5010</v>
@@ -3121,16 +3120,16 @@
         <v>45384</v>
       </c>
       <c r="B41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C41" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D41" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E41" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F41">
         <v>10300</v>
@@ -3142,10 +3141,10 @@
         <v>3</v>
       </c>
       <c r="I41" t="s">
+        <v>212</v>
+      </c>
+      <c r="J41" t="s">
         <v>216</v>
-      </c>
-      <c r="J41" t="s">
-        <v>220</v>
       </c>
       <c r="M41">
         <v>5010</v>
@@ -3165,16 +3164,16 @@
         <v>45384</v>
       </c>
       <c r="B42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C42" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D42" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E42" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F42">
         <v>10302</v>
@@ -3186,10 +3185,10 @@
         <v>2</v>
       </c>
       <c r="I42" t="s">
+        <v>212</v>
+      </c>
+      <c r="J42" t="s">
         <v>216</v>
-      </c>
-      <c r="J42" t="s">
-        <v>220</v>
       </c>
       <c r="M42">
         <v>5010</v>
@@ -3209,16 +3208,16 @@
         <v>45384</v>
       </c>
       <c r="B43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C43" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D43" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E43" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F43">
         <v>1183</v>
@@ -3230,10 +3229,10 @@
         <v>3</v>
       </c>
       <c r="I43" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J43" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="M43">
         <v>255</v>
@@ -3253,16 +3252,16 @@
         <v>45384</v>
       </c>
       <c r="B44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C44" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D44" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E44" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F44">
         <v>10299</v>
@@ -3274,10 +3273,10 @@
         <v>2</v>
       </c>
       <c r="I44" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J44" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="M44">
         <v>8783</v>
@@ -3297,16 +3296,16 @@
         <v>45389</v>
       </c>
       <c r="B45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C45" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D45" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E45" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F45">
         <v>1360</v>
@@ -3318,10 +3317,10 @@
         <v>8</v>
       </c>
       <c r="I45" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J45" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="M45">
         <v>270</v>
@@ -3341,16 +3340,16 @@
         <v>45409</v>
       </c>
       <c r="B46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C46" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D46" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E46" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F46">
         <v>10319</v>
@@ -3362,10 +3361,10 @@
         <v>3</v>
       </c>
       <c r="I46" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J46" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="M46">
         <v>9382</v>
@@ -3385,16 +3384,16 @@
         <v>45658</v>
       </c>
       <c r="B47" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C47" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D47" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="E47" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="F47">
         <v>288</v>
@@ -3407,10 +3406,10 @@
         <v>5</v>
       </c>
       <c r="I47" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="J47" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="M47">
         <v>58</v>
@@ -3430,16 +3429,16 @@
         <v>45660</v>
       </c>
       <c r="B48" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C48" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D48" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E48" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F48">
         <v>1183</v>
@@ -3451,10 +3450,10 @@
         <v>9</v>
       </c>
       <c r="I48" t="s">
+        <v>212</v>
+      </c>
+      <c r="J48" t="s">
         <v>216</v>
-      </c>
-      <c r="J48" t="s">
-        <v>220</v>
       </c>
       <c r="M48">
         <v>193</v>
@@ -3474,16 +3473,16 @@
         <v>45660</v>
       </c>
       <c r="B49" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C49" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D49" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="E49" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F49">
         <v>927</v>
@@ -3495,10 +3494,10 @@
         <v>4</v>
       </c>
       <c r="I49" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J49" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="M49">
         <v>662</v>
@@ -3518,16 +3517,16 @@
         <v>45662</v>
       </c>
       <c r="B50" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C50" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D50" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="E50" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F50">
         <v>927</v>
@@ -3540,10 +3539,10 @@
         <v>12</v>
       </c>
       <c r="I50" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J50" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="M50">
         <v>662</v>
@@ -3563,16 +3562,16 @@
         <v>45690</v>
       </c>
       <c r="B51" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C51" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="D51" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="E51" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="F51">
         <v>2665</v>
@@ -3584,10 +3583,10 @@
         <v>4</v>
       </c>
       <c r="I51" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J51" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="M51">
         <v>717</v>
@@ -3607,16 +3606,16 @@
         <v>45691</v>
       </c>
       <c r="B52" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="C52" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D52" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E52" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="F52">
         <v>1292</v>
@@ -3629,10 +3628,10 @@
         <v>10</v>
       </c>
       <c r="I52" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J52" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="M52">
         <v>622</v>
@@ -3652,16 +3651,16 @@
         <v>45707</v>
       </c>
       <c r="B53" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C53" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D53" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="E53" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="F53">
         <v>1143</v>
@@ -3673,10 +3672,10 @@
         <v>14</v>
       </c>
       <c r="I53" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J53" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="M53">
         <v>617</v>
@@ -3696,16 +3695,16 @@
         <v>45714</v>
       </c>
       <c r="B54" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C54" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D54" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="E54" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="F54">
         <v>3199</v>
@@ -3717,10 +3716,10 @@
         <v>7</v>
       </c>
       <c r="I54" t="s">
+        <v>212</v>
+      </c>
+      <c r="J54" t="s">
         <v>216</v>
-      </c>
-      <c r="J54" t="s">
-        <v>220</v>
       </c>
       <c r="M54">
         <v>2991</v>
@@ -3740,16 +3739,16 @@
         <v>45719</v>
       </c>
       <c r="B55" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C55" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D55" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E55" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F55">
         <v>3200</v>
@@ -3761,10 +3760,10 @@
         <v>4</v>
       </c>
       <c r="I55" t="s">
+        <v>212</v>
+      </c>
+      <c r="J55" t="s">
         <v>216</v>
-      </c>
-      <c r="J55" t="s">
-        <v>220</v>
       </c>
       <c r="M55">
         <v>1898</v>
@@ -3784,16 +3783,16 @@
         <v>45733</v>
       </c>
       <c r="B56" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C56" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D56" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="E56" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="F56">
         <v>3076</v>
@@ -3805,10 +3804,10 @@
         <v>7</v>
       </c>
       <c r="I56" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="J56" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M56">
         <v>1166</v>
@@ -3828,16 +3827,16 @@
         <v>45741</v>
       </c>
       <c r="B57" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C57" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D57" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="E57" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="F57">
         <v>967</v>
@@ -3849,10 +3848,10 @@
         <v>4</v>
       </c>
       <c r="I57" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="J57" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M57">
         <v>278</v>
@@ -3872,16 +3871,16 @@
         <v>45752</v>
       </c>
       <c r="B58" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C58" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D58" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="E58" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="F58">
         <v>2223</v>
@@ -3893,10 +3892,10 @@
         <v>3</v>
       </c>
       <c r="I58" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="J58" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M58">
         <v>174</v>
@@ -3916,16 +3915,16 @@
         <v>45754</v>
       </c>
       <c r="B59" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C59" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D59" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E59" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="F59">
         <v>1932</v>
@@ -3937,10 +3936,10 @@
         <v>2</v>
       </c>
       <c r="I59" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="J59" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M59">
         <v>787</v>
@@ -3960,16 +3959,16 @@
         <v>45782</v>
       </c>
       <c r="B60" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C60" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D60" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E60" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F60">
         <v>4230</v>
@@ -3981,10 +3980,10 @@
         <v>12</v>
       </c>
       <c r="I60" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="J60" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M60">
         <v>739</v>
@@ -4004,16 +4003,16 @@
         <v>45791</v>
       </c>
       <c r="B61" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C61" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D61" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="E61" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F61">
         <v>160</v>
@@ -4025,10 +4024,10 @@
         <v>14</v>
       </c>
       <c r="I61" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J61" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="M61">
         <v>95</v>
@@ -4048,16 +4047,16 @@
         <v>45795</v>
       </c>
       <c r="B62" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C62" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D62" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E62" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F62">
         <v>1033</v>
@@ -4069,10 +4068,10 @@
         <v>2</v>
       </c>
       <c r="I62" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="J62" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M62">
         <v>309</v>
@@ -4092,16 +4091,16 @@
         <v>45800</v>
       </c>
       <c r="B63" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C63" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D63" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E63" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="F63">
         <v>2705</v>
@@ -4113,10 +4112,10 @@
         <v>5</v>
       </c>
       <c r="I63" t="s">
+        <v>212</v>
+      </c>
+      <c r="J63" t="s">
         <v>216</v>
-      </c>
-      <c r="J63" t="s">
-        <v>220</v>
       </c>
       <c r="M63">
         <v>803</v>
@@ -4136,16 +4135,16 @@
         <v>45800</v>
       </c>
       <c r="B64" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C64" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D64" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E64" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="F64">
         <v>2706</v>
@@ -4157,10 +4156,10 @@
         <v>8</v>
       </c>
       <c r="I64" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J64" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="M64">
         <v>670</v>
@@ -4180,16 +4179,16 @@
         <v>45801</v>
       </c>
       <c r="B65" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="C65" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="D65" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="E65" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="F65">
         <v>1247</v>
@@ -4202,10 +4201,10 @@
         <v>3</v>
       </c>
       <c r="I65" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="J65" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="M65">
         <v>354</v>
@@ -4228,13 +4227,13 @@
         <v>44</v>
       </c>
       <c r="C66" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D66" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E66" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F66">
         <v>1036</v>
@@ -4246,10 +4245,10 @@
         <v>3</v>
       </c>
       <c r="I66" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="J66" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M66">
         <v>309</v>
@@ -4272,13 +4271,13 @@
         <v>45</v>
       </c>
       <c r="C67" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D67" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E67" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F67">
         <v>944</v>
@@ -4290,10 +4289,10 @@
         <v>37</v>
       </c>
       <c r="I67" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J67" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M67">
         <v>246</v>
@@ -4316,13 +4315,13 @@
         <v>46</v>
       </c>
       <c r="C68" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D68" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E68" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F68">
         <v>942</v>
@@ -4334,10 +4333,10 @@
         <v>4</v>
       </c>
       <c r="I68" t="s">
+        <v>212</v>
+      </c>
+      <c r="J68" t="s">
         <v>216</v>
-      </c>
-      <c r="J68" t="s">
-        <v>220</v>
       </c>
       <c r="M68">
         <v>54</v>
@@ -4360,13 +4359,13 @@
         <v>47</v>
       </c>
       <c r="C69" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D69" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E69" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F69">
         <v>3087</v>
@@ -4378,10 +4377,10 @@
         <v>3</v>
       </c>
       <c r="I69" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J69" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="M69">
         <v>348</v>
@@ -4404,13 +4403,13 @@
         <v>48</v>
       </c>
       <c r="C70" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D70" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E70" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F70">
         <v>121</v>
@@ -4422,16 +4421,16 @@
         <v>66</v>
       </c>
       <c r="I70" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J70" t="s">
+        <v>218</v>
+      </c>
+      <c r="K70" t="s">
         <v>222</v>
       </c>
-      <c r="K70" t="s">
-        <v>227</v>
-      </c>
       <c r="L70" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
@@ -4442,13 +4441,13 @@
         <v>49</v>
       </c>
       <c r="C71" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D71" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E71" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F71">
         <v>683</v>
@@ -4460,10 +4459,10 @@
         <v>3</v>
       </c>
       <c r="I71" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J71" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="M71">
         <v>223</v>
@@ -4486,13 +4485,13 @@
         <v>50</v>
       </c>
       <c r="C72" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D72" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E72" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F72">
         <v>167</v>
@@ -4504,13 +4503,13 @@
         <v>27</v>
       </c>
       <c r="I72" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J72" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="L72" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.2">
@@ -4521,13 +4520,13 @@
         <v>51</v>
       </c>
       <c r="C73" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D73" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E73" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F73">
         <v>8948</v>
@@ -4539,10 +4538,10 @@
         <v>4</v>
       </c>
       <c r="I73" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="J73" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.2">
@@ -4553,13 +4552,13 @@
         <v>52</v>
       </c>
       <c r="C74" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D74" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E74" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F74">
         <v>8948</v>
@@ -4571,10 +4570,10 @@
         <v>2</v>
       </c>
       <c r="I74" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="J74" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="M74">
         <v>6332</v>
@@ -4597,13 +4596,13 @@
         <v>53</v>
       </c>
       <c r="C75" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D75" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E75" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F75">
         <v>708</v>
@@ -4615,13 +4614,13 @@
         <v>33</v>
       </c>
       <c r="I75" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J75" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="K75" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M75">
         <v>660</v>
@@ -4637,53 +4636,53 @@
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A76" s="2">
-        <v>45810</v>
+      <c r="A76" s="5">
+        <v>45674</v>
       </c>
       <c r="B76" t="s">
-        <v>54</v>
+        <v>305</v>
       </c>
       <c r="C76" t="s">
-        <v>109</v>
+        <v>306</v>
       </c>
       <c r="D76" t="s">
-        <v>155</v>
+        <v>307</v>
       </c>
       <c r="E76" t="s">
-        <v>202</v>
+        <v>308</v>
       </c>
       <c r="F76">
-        <v>243</v>
+        <v>966</v>
       </c>
       <c r="G76">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="H76">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I76" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="J76" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="M76">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="N76">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O76">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="P76">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P76" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P79">
-      <sortCondition ref="A1:A79"/>
+  <autoFilter ref="A1:P75" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P78">
+      <sortCondition ref="A1:A78"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>